<commit_message>
Bug but will release...
</commit_message>
<xml_diff>
--- a/Strings.xlsx
+++ b/Strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WindowsFile\TheOtherRolesRework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACD78A7-4DA0-4EC6-AC61-A4789B03F24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170105B-4438-4083-843D-5DD6CAEAE004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2673" uniqueCount="2461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="2452">
   <si>
     <t>English</t>
   </si>
@@ -7010,39 +7010,6 @@
     <t>ghostsSeeInformation</t>
   </si>
   <si>
-    <t>Ghosts See Tasks &amp; Other Info</t>
-  </si>
-  <si>
-    <t>灵魂可见任务和其他信息</t>
-  </si>
-  <si>
-    <t>ghostsSeeVotes</t>
-  </si>
-  <si>
-    <t>Ghosts Can See Votes</t>
-  </si>
-  <si>
-    <t>灵魂可见投票结果</t>
-  </si>
-  <si>
-    <t>ghostsSeeRoles</t>
-  </si>
-  <si>
-    <t>Ghosts Can See Roles</t>
-  </si>
-  <si>
-    <t>灵魂可见玩家职业</t>
-  </si>
-  <si>
-    <t>ghostsSeeModifier</t>
-  </si>
-  <si>
-    <t>Ghosts Can Additionally See Modifier</t>
-  </si>
-  <si>
-    <t>灵魂可见附加职业</t>
-  </si>
-  <si>
     <t>showRoleSummary</t>
   </si>
   <si>
@@ -7052,15 +7019,6 @@
     <t>显示职业总结</t>
   </si>
   <si>
-    <t>showLighterDarker</t>
-  </si>
-  <si>
-    <t>Show Lighter / Darker</t>
-  </si>
-  <si>
-    <t>显示颜色深浅</t>
-  </si>
-  <si>
     <t>enableSoundEffects</t>
   </si>
   <si>
@@ -7068,15 +7026,6 @@
   </si>
   <si>
     <t>启用模组音效</t>
-  </si>
-  <si>
-    <t>showVentsOnMap</t>
-  </si>
-  <si>
-    <t>Show Vents On Map</t>
-  </si>
-  <si>
-    <t>在地图上显示管道位置</t>
   </si>
   <si>
     <t>showChatNotifications</t>
@@ -7731,6 +7680,38 @@
   </si>
   <si>
     <t>和平之鸽重置了你的冷却时间！</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ghosts See More Infos</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵魂可见更多信息</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable Dark Mode</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>enableDarkMode</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用深色模式</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instead Dark Mod Of Role Color</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>insteadRoleColor</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>启用职业颜色代替深色模式</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -8284,8 +8265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q939"/>
   <sheetViews>
-    <sheetView topLeftCell="A879" workbookViewId="0">
-      <selection activeCell="O889" sqref="O889"/>
+    <sheetView tabSelected="1" topLeftCell="A739" workbookViewId="0">
+      <selection activeCell="A753" sqref="A753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14"/>
@@ -9065,7 +9046,7 @@
         <v>196</v>
       </c>
       <c r="O79" s="13" t="s">
-        <v>2294</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="80" spans="1:15">
@@ -9792,7 +9773,7 @@
       </c>
       <c r="C152" s="4"/>
       <c r="O152" s="13" t="s">
-        <v>2303</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="153" spans="1:15">
@@ -10245,7 +10226,7 @@
     </row>
     <row r="195" spans="1:15">
       <c r="A195" s="16" t="s">
-        <v>2321</v>
+        <v>2304</v>
       </c>
       <c r="B195" s="4" t="s">
         <v>444</v>
@@ -10257,7 +10238,7 @@
     </row>
     <row r="196" spans="1:15">
       <c r="A196" s="16" t="s">
-        <v>2323</v>
+        <v>2306</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>446</v>
@@ -10352,38 +10333,38 @@
     </row>
     <row r="205" spans="1:15">
       <c r="A205" s="16" t="s">
-        <v>2320</v>
+        <v>2303</v>
       </c>
       <c r="B205" s="16" t="s">
-        <v>2325</v>
+        <v>2308</v>
       </c>
       <c r="C205" s="4"/>
       <c r="O205" s="15" t="s">
-        <v>2314</v>
+        <v>2297</v>
       </c>
     </row>
     <row r="206" spans="1:15">
       <c r="A206" s="16" t="s">
-        <v>2322</v>
+        <v>2305</v>
       </c>
       <c r="B206" s="4" t="s">
-        <v>2326</v>
+        <v>2309</v>
       </c>
       <c r="C206" s="4"/>
       <c r="O206" s="15" t="s">
-        <v>2315</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="207" spans="1:15">
       <c r="A207" s="16" t="s">
-        <v>2324</v>
+        <v>2307</v>
       </c>
       <c r="B207" s="16" t="s">
-        <v>2330</v>
+        <v>2313</v>
       </c>
       <c r="C207" s="4"/>
       <c r="O207" s="15" t="s">
-        <v>2316</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="208" spans="1:15">
@@ -10394,38 +10375,38 @@
     </row>
     <row r="209" spans="1:16">
       <c r="A209" s="16" t="s">
-        <v>2332</v>
+        <v>2315</v>
       </c>
       <c r="B209" s="16" t="s">
-        <v>2327</v>
+        <v>2310</v>
       </c>
       <c r="C209" s="4"/>
       <c r="O209" s="15" t="s">
-        <v>2317</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="210" spans="1:16">
       <c r="A210" s="16" t="s">
-        <v>2331</v>
+        <v>2314</v>
       </c>
       <c r="B210" s="16" t="s">
-        <v>2328</v>
+        <v>2311</v>
       </c>
       <c r="C210" s="4"/>
       <c r="O210" s="15" t="s">
-        <v>2318</v>
+        <v>2301</v>
       </c>
     </row>
     <row r="211" spans="1:16">
       <c r="A211" s="4" t="s">
-        <v>2333</v>
+        <v>2316</v>
       </c>
       <c r="B211" s="16" t="s">
-        <v>2329</v>
+        <v>2312</v>
       </c>
       <c r="C211" s="4"/>
       <c r="O211" s="15" t="s">
-        <v>2319</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="212" spans="1:16">
@@ -10436,38 +10417,38 @@
     </row>
     <row r="213" spans="1:16">
       <c r="A213" s="16" t="s">
-        <v>2357</v>
+        <v>2340</v>
       </c>
       <c r="B213" s="16" t="s">
-        <v>2358</v>
+        <v>2341</v>
       </c>
       <c r="C213" s="4"/>
       <c r="O213" s="15" t="s">
-        <v>2359</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="214" spans="1:16">
       <c r="A214" s="16" t="s">
-        <v>2360</v>
+        <v>2343</v>
       </c>
       <c r="B214" s="16" t="s">
-        <v>2362</v>
+        <v>2345</v>
       </c>
       <c r="C214" s="4"/>
       <c r="O214" s="15" t="s">
-        <v>2364</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="215" spans="1:16">
       <c r="A215" s="16" t="s">
-        <v>2361</v>
+        <v>2344</v>
       </c>
       <c r="B215" s="16" t="s">
-        <v>2363</v>
+        <v>2346</v>
       </c>
       <c r="C215" s="4"/>
       <c r="O215" s="15" t="s">
-        <v>2365</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="216" spans="1:16">
@@ -10478,111 +10459,111 @@
     </row>
     <row r="217" spans="1:16">
       <c r="A217" s="16" t="s">
-        <v>2366</v>
+        <v>2349</v>
       </c>
       <c r="B217" s="16" t="s">
-        <v>2371</v>
+        <v>2354</v>
       </c>
       <c r="C217" s="4"/>
       <c r="O217" s="15" t="s">
-        <v>2370</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="218" spans="1:16">
       <c r="A218" s="16" t="s">
-        <v>2372</v>
+        <v>2355</v>
       </c>
       <c r="B218" s="16" t="s">
-        <v>2373</v>
+        <v>2356</v>
       </c>
       <c r="C218" s="4"/>
       <c r="O218" s="15" t="s">
-        <v>2374</v>
+        <v>2357</v>
       </c>
     </row>
     <row r="219" spans="1:16">
       <c r="A219" s="16" t="s">
-        <v>2375</v>
+        <v>2358</v>
       </c>
       <c r="B219" s="16" t="s">
-        <v>2376</v>
+        <v>2359</v>
       </c>
       <c r="C219" s="4"/>
       <c r="O219" s="15" t="s">
-        <v>2377</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="220" spans="1:16">
       <c r="A220" s="16" t="s">
-        <v>2379</v>
+        <v>2362</v>
       </c>
       <c r="B220" s="16" t="s">
-        <v>2378</v>
+        <v>2361</v>
       </c>
       <c r="C220" s="4"/>
       <c r="O220" s="15" t="s">
-        <v>2380</v>
+        <v>2363</v>
       </c>
     </row>
     <row r="221" spans="1:16">
       <c r="A221" s="16" t="s">
-        <v>2381</v>
+        <v>2364</v>
       </c>
       <c r="B221" s="16" t="s">
-        <v>2382</v>
+        <v>2365</v>
       </c>
       <c r="C221" s="4"/>
       <c r="O221" s="15" t="s">
-        <v>2383</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="222" spans="1:16">
       <c r="A222" s="16" t="s">
-        <v>2384</v>
+        <v>2367</v>
       </c>
       <c r="B222" s="16" t="s">
-        <v>2385</v>
+        <v>2368</v>
       </c>
       <c r="C222" s="4"/>
       <c r="O222" s="15" t="s">
-        <v>2386</v>
+        <v>2369</v>
       </c>
     </row>
     <row r="223" spans="1:16">
       <c r="A223" s="16" t="s">
-        <v>2387</v>
+        <v>2370</v>
       </c>
       <c r="B223" s="16" t="s">
-        <v>2388</v>
+        <v>2371</v>
       </c>
       <c r="C223" s="4"/>
       <c r="O223" s="15" t="s">
-        <v>2389</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="224" spans="1:16">
       <c r="A224" s="16" t="s">
-        <v>2390</v>
+        <v>2373</v>
       </c>
       <c r="B224" s="16" t="s">
-        <v>2391</v>
+        <v>2374</v>
       </c>
       <c r="C224" s="4"/>
       <c r="O224" s="13" t="s">
-        <v>2392</v>
+        <v>2375</v>
       </c>
       <c r="P224" s="15"/>
     </row>
     <row r="225" spans="1:16">
       <c r="A225" s="16" t="s">
-        <v>2393</v>
+        <v>2376</v>
       </c>
       <c r="B225" s="16" t="s">
-        <v>2394</v>
+        <v>2377</v>
       </c>
       <c r="C225" s="4"/>
       <c r="O225" s="13" t="s">
-        <v>2395</v>
+        <v>2378</v>
       </c>
       <c r="P225" s="15"/>
     </row>
@@ -11796,13 +11777,13 @@
     </row>
     <row r="347" spans="1:15">
       <c r="A347" s="9" t="s">
-        <v>2338</v>
+        <v>2321</v>
       </c>
       <c r="B347" s="14" t="s">
-        <v>2339</v>
+        <v>2322</v>
       </c>
       <c r="O347" s="16" t="s">
-        <v>2340</v>
+        <v>2323</v>
       </c>
     </row>
     <row r="348" spans="1:15">
@@ -11959,13 +11940,13 @@
     </row>
     <row r="363" spans="1:15">
       <c r="A363" s="14" t="s">
-        <v>2341</v>
+        <v>2324</v>
       </c>
       <c r="B363" s="14" t="s">
-        <v>2342</v>
+        <v>2325</v>
       </c>
       <c r="O363" s="13" t="s">
-        <v>2343</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="364" spans="1:15">
@@ -13489,7 +13470,7 @@
         <v>1133</v>
       </c>
       <c r="O520" s="13" t="s">
-        <v>2295</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="521" spans="1:15">
@@ -13628,7 +13609,7 @@
     </row>
     <row r="537" spans="1:15">
       <c r="A537" s="14" t="s">
-        <v>2304</v>
+        <v>2287</v>
       </c>
       <c r="B537" s="9" t="s">
         <v>1162</v>
@@ -14336,7 +14317,7 @@
         <v>1322</v>
       </c>
       <c r="O614" s="13" t="s">
-        <v>2306</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="615" spans="1:15">
@@ -15297,7 +15278,7 @@
     </row>
     <row r="713" spans="1:15">
       <c r="A713" s="14" t="s">
-        <v>2305</v>
+        <v>2288</v>
       </c>
       <c r="B713" s="9" t="s">
         <v>1557</v>
@@ -15378,24 +15359,24 @@
     </row>
     <row r="722" spans="1:15">
       <c r="A722" s="14" t="s">
-        <v>2297</v>
+        <v>2280</v>
       </c>
       <c r="B722" s="14" t="s">
-        <v>2298</v>
+        <v>2281</v>
       </c>
       <c r="O722" s="13" t="s">
-        <v>2299</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="723" spans="1:15">
       <c r="A723" s="1" t="s">
-        <v>2300</v>
+        <v>2283</v>
       </c>
       <c r="B723" s="13" t="s">
-        <v>2301</v>
+        <v>2284</v>
       </c>
       <c r="O723" s="13" t="s">
-        <v>2302</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="725" spans="1:15">
@@ -15406,7 +15387,7 @@
         <v>1578</v>
       </c>
       <c r="O725" s="13" t="s">
-        <v>2296</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="726" spans="1:15">
@@ -15466,11 +15447,11 @@
     </row>
     <row r="733" spans="1:15">
       <c r="A733" s="13" t="s">
-        <v>2402</v>
+        <v>2385</v>
       </c>
       <c r="B733" s="13"/>
       <c r="O733" s="13" t="s">
-        <v>2412</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="734" spans="1:15">
@@ -15478,102 +15459,102 @@
     </row>
     <row r="735" spans="1:15">
       <c r="A735" s="13" t="s">
-        <v>2410</v>
+        <v>2393</v>
       </c>
       <c r="B735" s="13" t="s">
-        <v>2435</v>
+        <v>2418</v>
       </c>
       <c r="C735" s="13"/>
       <c r="O735" s="13" t="s">
-        <v>2413</v>
+        <v>2396</v>
       </c>
     </row>
     <row r="736" spans="1:15">
       <c r="A736" s="13" t="s">
-        <v>2411</v>
+        <v>2394</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>2434</v>
+        <v>2417</v>
       </c>
       <c r="O736" s="13" t="s">
-        <v>2414</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="738" spans="1:15">
       <c r="A738" s="13" t="s">
-        <v>2408</v>
+        <v>2391</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>2420</v>
+        <v>2403</v>
       </c>
       <c r="O738" s="13" t="s">
-        <v>2421</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="739" spans="1:15">
       <c r="A739" s="1" t="s">
-        <v>2403</v>
+        <v>2386</v>
       </c>
       <c r="B739" s="13" t="s">
-        <v>2425</v>
+        <v>2408</v>
       </c>
       <c r="O739" s="13" t="s">
-        <v>2428</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="740" spans="1:15">
       <c r="A740" s="1" t="s">
-        <v>2404</v>
+        <v>2387</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>2422</v>
+        <v>2405</v>
       </c>
       <c r="O740" s="13" t="s">
-        <v>2429</v>
+        <v>2412</v>
       </c>
     </row>
     <row r="741" spans="1:15">
       <c r="A741" s="1" t="s">
-        <v>2405</v>
+        <v>2388</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>2423</v>
+        <v>2406</v>
       </c>
       <c r="O741" s="13" t="s">
-        <v>2430</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="742" spans="1:15">
       <c r="A742" s="1" t="s">
-        <v>2406</v>
+        <v>2389</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>2424</v>
+        <v>2407</v>
       </c>
       <c r="O742" s="13" t="s">
-        <v>2431</v>
+        <v>2414</v>
       </c>
     </row>
     <row r="743" spans="1:15">
       <c r="A743" s="1" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B743" s="13" t="s">
         <v>2409</v>
       </c>
-      <c r="B743" s="13" t="s">
-        <v>2426</v>
-      </c>
       <c r="O743" s="13" t="s">
-        <v>2432</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="744" spans="1:15">
       <c r="A744" s="1" t="s">
-        <v>2407</v>
+        <v>2390</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>2427</v>
+        <v>2410</v>
       </c>
       <c r="O744" s="13" t="s">
-        <v>2433</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="745" spans="1:15">
@@ -15581,13 +15562,13 @@
     </row>
     <row r="746" spans="1:15">
       <c r="A746" s="13" t="s">
-        <v>2436</v>
+        <v>2419</v>
       </c>
       <c r="B746" s="13" t="s">
-        <v>2441</v>
+        <v>2424</v>
       </c>
       <c r="O746" s="13" t="s">
-        <v>2446</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="747" spans="1:15">
@@ -15595,24 +15576,24 @@
     </row>
     <row r="748" spans="1:15">
       <c r="A748" s="13" t="s">
-        <v>2437</v>
+        <v>2420</v>
       </c>
       <c r="B748" s="13" t="s">
-        <v>2443</v>
+        <v>2426</v>
       </c>
       <c r="O748" s="13" t="s">
-        <v>2447</v>
+        <v>2430</v>
       </c>
     </row>
     <row r="749" spans="1:15">
       <c r="A749" s="13" t="s">
-        <v>2438</v>
+        <v>2421</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>2442</v>
+        <v>2425</v>
       </c>
       <c r="O749" s="13" t="s">
-        <v>2451</v>
+        <v>2434</v>
       </c>
     </row>
     <row r="750" spans="1:15">
@@ -15620,35 +15601,35 @@
     </row>
     <row r="751" spans="1:15">
       <c r="A751" s="13" t="s">
-        <v>2439</v>
+        <v>2422</v>
       </c>
       <c r="B751" s="13" t="s">
-        <v>2444</v>
+        <v>2427</v>
       </c>
       <c r="O751" s="13" t="s">
-        <v>2448</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="752" spans="1:15">
       <c r="A752" s="1" t="s">
-        <v>2440</v>
+        <v>2423</v>
       </c>
       <c r="B752" s="13" t="s">
-        <v>2445</v>
+        <v>2428</v>
       </c>
       <c r="O752" s="13" t="s">
-        <v>2452</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="753" spans="1:15">
       <c r="A753" s="13" t="s">
-        <v>2449</v>
+        <v>2432</v>
       </c>
       <c r="B753" s="13" t="s">
-        <v>2450</v>
+        <v>2433</v>
       </c>
       <c r="O753" s="13" t="s">
-        <v>2453</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="758" spans="1:15">
@@ -16126,29 +16107,29 @@
     </row>
     <row r="809" spans="1:15">
       <c r="A809" s="13" t="s">
-        <v>2308</v>
+        <v>2291</v>
       </c>
       <c r="B809" s="13" t="s">
-        <v>2311</v>
+        <v>2294</v>
       </c>
       <c r="O809" s="13" t="s">
-        <v>2312</v>
+        <v>2295</v>
       </c>
     </row>
     <row r="810" spans="1:15">
       <c r="A810" s="13" t="s">
-        <v>2309</v>
+        <v>2292</v>
       </c>
       <c r="B810" s="13" t="s">
-        <v>2310</v>
+        <v>2293</v>
       </c>
       <c r="O810" s="13" t="s">
-        <v>2313</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="812" spans="1:15">
       <c r="A812" s="13" t="s">
-        <v>2307</v>
+        <v>2290</v>
       </c>
       <c r="B812" s="1" t="s">
         <v>1717</v>
@@ -16522,13 +16503,13 @@
     </row>
     <row r="858" spans="1:15">
       <c r="A858" s="1" t="s">
-        <v>2417</v>
+        <v>2400</v>
       </c>
       <c r="B858" s="13" t="s">
-        <v>2418</v>
+        <v>2401</v>
       </c>
       <c r="O858" s="13" t="s">
-        <v>2419</v>
+        <v>2402</v>
       </c>
     </row>
     <row r="860" spans="1:15">
@@ -16775,7 +16756,7 @@
     </row>
     <row r="885" spans="1:15">
       <c r="A885" s="1" t="s">
-        <v>2356</v>
+        <v>2339</v>
       </c>
       <c r="B885" s="1" t="s">
         <v>1881</v>
@@ -16808,13 +16789,13 @@
     </row>
     <row r="889" spans="1:15">
       <c r="A889" s="13" t="s">
-        <v>2458</v>
+        <v>2441</v>
       </c>
       <c r="B889" s="13" t="s">
-        <v>2459</v>
+        <v>2442</v>
       </c>
       <c r="O889" s="13" t="s">
-        <v>2460</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="890" spans="1:15">
@@ -17248,36 +17229,36 @@
     </row>
     <row r="937" spans="1:16">
       <c r="A937" s="13" t="s">
-        <v>2334</v>
+        <v>2317</v>
       </c>
       <c r="B937" s="13" t="s">
-        <v>2335</v>
+        <v>2318</v>
       </c>
       <c r="O937" s="13" t="s">
-        <v>2336</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="938" spans="1:16">
       <c r="A938" s="13" t="s">
-        <v>2401</v>
+        <v>2384</v>
       </c>
       <c r="B938" s="13" t="s">
-        <v>2399</v>
+        <v>2382</v>
       </c>
       <c r="O938" s="13" t="s">
-        <v>2400</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="939" spans="1:16">
       <c r="A939" s="16" t="s">
-        <v>2396</v>
+        <v>2379</v>
       </c>
       <c r="B939" s="16" t="s">
-        <v>2397</v>
+        <v>2380</v>
       </c>
       <c r="C939" s="4"/>
       <c r="O939" s="1" t="s">
-        <v>2398</v>
+        <v>2381</v>
       </c>
       <c r="P939" s="15"/>
     </row>
@@ -17293,7 +17274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
@@ -17868,46 +17849,46 @@
     </row>
     <row r="48" spans="1:15">
       <c r="A48" s="13" t="s">
-        <v>2337</v>
+        <v>2320</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>2310</v>
+        <v>2293</v>
       </c>
       <c r="O48" s="13" t="s">
-        <v>2313</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="A49" s="13" t="s">
-        <v>2367</v>
+        <v>2350</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>2368</v>
+        <v>2351</v>
       </c>
       <c r="O49" s="13" t="s">
-        <v>2369</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="50" spans="1:15">
       <c r="A50" s="13" t="s">
-        <v>2454</v>
+        <v>2437</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>2415</v>
+        <v>2398</v>
       </c>
       <c r="O50" s="13" t="s">
-        <v>2416</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="51" spans="1:15">
       <c r="A51" s="13" t="s">
-        <v>2455</v>
+        <v>2438</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>2456</v>
+        <v>2439</v>
       </c>
       <c r="O51" s="13" t="s">
-        <v>2457</v>
+        <v>2440</v>
       </c>
     </row>
   </sheetData>
@@ -17921,7 +17902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -19275,35 +19256,35 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="13" t="s">
-        <v>2347</v>
+        <v>2330</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>2348</v>
+        <v>2331</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>2349</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="13" t="s">
-        <v>2350</v>
+        <v>2333</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>2351</v>
+        <v>2334</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>2352</v>
+        <v>2335</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="13" t="s">
-        <v>2353</v>
+        <v>2336</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>2355</v>
+        <v>2338</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>2354</v>
+        <v>2337</v>
       </c>
     </row>
   </sheetData>
@@ -19314,10 +19295,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14"/>
@@ -19418,110 +19399,77 @@
       <c r="A5" s="1" t="s">
         <v>2267</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2268</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>2269</v>
+      <c r="B5" s="13" t="s">
+        <v>2444</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>2445</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>2270</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>2271</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>2272</v>
-      </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
-        <v>2273</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2274</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>2275</v>
+      <c r="A7" s="13" t="s">
+        <v>2450</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>2449</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>2451</v>
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="1" t="s">
-        <v>2276</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2277</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>2278</v>
+      <c r="A8" s="13" t="s">
+        <v>2447</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>2446</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>2448</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
-        <v>2279</v>
+        <v>2271</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2280</v>
+        <v>2272</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>2281</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
-        <v>2282</v>
+        <v>2274</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2283</v>
+        <v>2275</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>2284</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1" t="s">
-        <v>2285</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>2286</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>2287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="1" t="s">
-        <v>2288</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>2289</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>2290</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="1" t="s">
-        <v>2291</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2292</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>2293</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="13" t="s">
-        <v>2344</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>2345</v>
-      </c>
-      <c r="O14" s="13" t="s">
-        <v>2346</v>
+      <c r="A11" s="13" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>2328</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>2329</v>
       </c>
     </row>
   </sheetData>
@@ -19531,6 +19479,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <pixelatorList sheetStid="1"/>
+  <pixelatorList sheetStid="2"/>
+  <pixelatorList sheetStid="3"/>
+  <pixelatorList sheetStid="4"/>
+  <pixelatorList sheetStid="5"/>
+  <pixelatorList sheetStid="6"/>
+</pixelators>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <woProps xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <woSheetsProps>
     <woSheetProps sheetStid="1" interlineOnOff="0" interlineColor="0" isDbSheet="0" isDashBoardSheet="0" isDbDashBoardSheet="0" isFlexPaperSheet="0">
@@ -19572,25 +19531,14 @@
 </woProps>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<pixelators xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <pixelatorList sheetStid="1"/>
-  <pixelatorList sheetStid="2"/>
-  <pixelatorList sheetStid="3"/>
-  <pixelatorList sheetStid="4"/>
-  <pixelatorList sheetStid="5"/>
-  <pixelatorList sheetStid="6"/>
-</pixelators>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224D003E-15C9-4FFE-AB16-9E66474EAE4E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C82605-B75B-4693-9329-32AAD527C692}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>